<commit_message>
Création du create, getOne et getAll Post API
</commit_message>
<xml_diff>
--- a/Structure BDD.xlsx
+++ b/Structure BDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Formation Développeur Web\Git\P7_Aubert_Martin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFBA1EB1-E732-490C-A755-8186B39D1AE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B50BCBA-C5F4-4A47-8A47-A5A9F5018137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ADEC320F-E610-47DA-81E8-D01497374C73}"/>
+    <workbookView xWindow="1275" yWindow="300" windowWidth="27525" windowHeight="15300" xr2:uid="{ADEC320F-E610-47DA-81E8-D01497374C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -77,18 +77,6 @@
     <t>user_post</t>
   </si>
   <si>
-    <t>Commentaire</t>
-  </si>
-  <si>
-    <t>comentaire_post</t>
-  </si>
-  <si>
-    <t>date_commentaire</t>
-  </si>
-  <si>
-    <t>user_commentaire</t>
-  </si>
-  <si>
     <t>Like</t>
   </si>
   <si>
@@ -96,6 +84,21 @@
   </si>
   <si>
     <t>user_like</t>
+  </si>
+  <si>
+    <t>date_comment</t>
+  </si>
+  <si>
+    <t>user_comment</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>comment_post</t>
+  </si>
+  <si>
+    <t>like_post</t>
   </si>
 </sst>
 </file>
@@ -7690,6 +7693,1136 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>99384</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Groupe 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{310C4FFC-23EC-4FAC-95F8-7A309BA79968}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="12849225" y="695325"/>
+          <a:ext cx="4076700" cy="642309"/>
+          <a:chOff x="1801731" y="626789"/>
+          <a:chExt cx="1284619" cy="642309"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Rectangle : coins arrondis 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{403F25F4-736C-4A07-88BC-630FA92994D6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1801731" y="626789"/>
+            <a:ext cx="1284619" cy="642309"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Rectangle : coins arrondis 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12AD23C7-337D-4481-AAD4-BD0F450A9F8E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1820544" y="645602"/>
+            <a:ext cx="1246993" cy="604683"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8255" tIns="8255" rIns="8255" bIns="8255" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>User.id</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>74944</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>127959</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Groupe 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F7490EB-DE5C-403A-9733-3B9C3A378873}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="12849225" y="1314450"/>
+          <a:ext cx="1284619" cy="642309"/>
+          <a:chOff x="1801731" y="626789"/>
+          <a:chExt cx="1284619" cy="642309"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle : coins arrondis 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94FEA082-3FC7-49E4-85A7-B8AE4991EA8D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1801731" y="626789"/>
+            <a:ext cx="1284619" cy="642309"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle : coins arrondis 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E85FE22C-584D-492E-97DB-C803BCFDFD83}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1820544" y="645602"/>
+            <a:ext cx="1246993" cy="604683"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8255" tIns="8255" rIns="8255" bIns="8255" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>Post</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>user_post</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>684544</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>127959</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="11" name="Groupe 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD3D0A1A-B918-4D75-9F0A-05A92E766A86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="14220825" y="1314450"/>
+          <a:ext cx="1284619" cy="642309"/>
+          <a:chOff x="1801731" y="626789"/>
+          <a:chExt cx="1284619" cy="642309"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Rectangle : coins arrondis 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA1502ED-453B-4DFB-AB38-2493DC249E3F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1801731" y="626789"/>
+            <a:ext cx="1284619" cy="642309"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rectangle : coins arrondis 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{749C3017-CBDB-4A71-9E0B-3A9D8980BD5F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1820544" y="645602"/>
+            <a:ext cx="1246993" cy="604683"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8255" tIns="8255" rIns="8255" bIns="8255" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>Comment</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>user_comment</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>579769</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>127959</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="14" name="Groupe 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1E3A5A7-4B59-41AF-AC2F-E1A784416BAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="15640050" y="1314450"/>
+          <a:ext cx="1284619" cy="642309"/>
+          <a:chOff x="1801731" y="626789"/>
+          <a:chExt cx="1284619" cy="642309"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="Rectangle : coins arrondis 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA55FF1-4025-49AF-A1D5-4237A688383C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1801731" y="626789"/>
+            <a:ext cx="1284619" cy="642309"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Rectangle : coins arrondis 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22D4266C-86DA-47AD-8637-0CE2E4FE7F7E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1820544" y="645602"/>
+            <a:ext cx="1246993" cy="604683"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8255" tIns="8255" rIns="8255" bIns="8255" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>Like</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>user_like</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>118434</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="17" name="Groupe 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{890C1347-8E3B-41E8-8D45-A12CBE9E7AAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13630275" y="2638425"/>
+          <a:ext cx="2886075" cy="642309"/>
+          <a:chOff x="1801731" y="626789"/>
+          <a:chExt cx="1284619" cy="642309"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="Rectangle : coins arrondis 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253B2BAF-BC1C-4B9E-8AF7-788341EAEAD1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1801731" y="626789"/>
+            <a:ext cx="1284619" cy="642309"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="Rectangle : coins arrondis 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7839DB0B-0FA3-42EE-91DF-249DB3FD894D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1820544" y="645602"/>
+            <a:ext cx="1246993" cy="604683"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8255" tIns="8255" rIns="8255" bIns="8255" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>Post</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>id</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4134</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="24" name="Groupe 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2664CA6A-551B-4E2B-9801-683FB0144233}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13639800" y="3286125"/>
+          <a:ext cx="1428750" cy="642309"/>
+          <a:chOff x="1801731" y="626789"/>
+          <a:chExt cx="1284619" cy="642309"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="Rectangle : coins arrondis 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D2B0F87-8C0A-409D-BFDF-1C88E33B154F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1801731" y="626789"/>
+            <a:ext cx="1284619" cy="642309"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="Rectangle : coins arrondis 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB7463EE-22A9-4E31-98CE-04581560BE7F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1820544" y="645602"/>
+            <a:ext cx="1246993" cy="604683"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8255" tIns="8255" rIns="8255" bIns="8255" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>Comment</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>comment_post</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4134</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="Groupe 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49D68CAB-DECC-42B6-9D11-9880C914DF0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="15068550" y="3286125"/>
+          <a:ext cx="1428750" cy="642309"/>
+          <a:chOff x="1801731" y="626789"/>
+          <a:chExt cx="1284619" cy="642309"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="Rectangle : coins arrondis 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F91D7275-19C3-4868-AD44-83B7494B6A5D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1801731" y="626789"/>
+            <a:ext cx="1284619" cy="642309"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="Rectangle : coins arrondis 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6F00ED0-8CCE-45B5-9A89-E602BE73075A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1820544" y="645602"/>
+            <a:ext cx="1246993" cy="604683"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8255" tIns="8255" rIns="8255" bIns="8255" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>Like</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+              <a:lnSpc>
+                <a:spcPct val="90000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPct val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPct val="35000"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1300" kern="1200"/>
+              <a:t>like_post</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7992,8 +9125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1411A4-4559-4E64-AADD-4E1EC0CB1936}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8011,10 +9144,10 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -8039,10 +9172,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -8053,10 +9186,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -8067,9 +9200,11 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">

</xml_diff>